<commit_message>
upate kernel bugs, PS:remove one false positive
</commit_message>
<xml_diff>
--- a/kernel_bugs/number_of_yeas.xlsx
+++ b/kernel_bugs/number_of_yeas.xlsx
@@ -29,7 +29,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -42,6 +42,13 @@
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -65,8 +72,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -350,7 +358,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -391,8 +399,8 @@
       <c r="A5">
         <v>2014</v>
       </c>
-      <c r="B5">
-        <v>148</v>
+      <c r="B5" s="1">
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -497,12 +505,12 @@
       </c>
       <c r="B18">
         <f>SUM(B1:B17)</f>
-        <v>2188</v>
+        <v>2187</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:B36">
-    <sortCondition descending="1" ref="A1"/>
+  <sortState ref="A20:B36">
+    <sortCondition descending="1" ref="A20"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>